<commit_message>
Revert "Merge pull request #1 from FWSquatch/2score"
This reverts commit 6f4fff4dd0ecc68c7ab9c3f2f6d37b7ce72cb347, reversing
changes made to 1b1c13ccb0db5a605117cfaf4a6177180caa3952.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="127">
   <si>
     <t xml:space="preserve">#Vulnerability</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">gooduser</t>
   </si>
   <si>
-    <t xml:space="preserve">brubble</t>
+    <t xml:space="preserve">jperalta</t>
   </si>
   <si>
     <t xml:space="preserve">Essential user has been removed!</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">newuser</t>
   </si>
   <si>
-    <t xml:space="preserve">bambam</t>
+    <t xml:space="preserve">nscully</t>
   </si>
   <si>
     <t xml:space="preserve">User nscully has been added.</t>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t xml:space="preserve">removefromcron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jperalta</t>
   </si>
   <si>
     <t xml:space="preserve">hello</t>
@@ -590,19 +587,19 @@
   </sheetPr>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="54.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,10 +1505,10 @@
         <v>116</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>108</v>
@@ -1520,7 +1517,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,13 +1540,13 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>108</v>
@@ -1558,7 +1555,7 @@
         <v>7</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,7 +1563,7 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
@@ -1588,13 +1585,13 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E53" s="2" t="n">
         <v>10</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
@@ -1620,23 +1617,23 @@
         <v>87</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>10</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Revert "Revert "Merge pull request #1 from FWSquatch/2score""
This reverts commit 4606a3eb1077f4c997881c70b9d4ce96b88a4d05.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="128">
   <si>
     <t xml:space="preserve">#Vulnerability</t>
   </si>
@@ -58,319 +58,322 @@
     <t xml:space="preserve">gooduser</t>
   </si>
   <si>
+    <t xml:space="preserve">brubble</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essential user has been removed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users who should be added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newuser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bambam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User nscully has been added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To disable this, delete the entire row below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkfirewall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firewall is enabled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text to remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#File to remove it from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removefromfile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allow-guest=true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/etc/lightdm/lightdm.conf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guest account disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text to add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#File to add it to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addtofile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PermitRootLogin no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/etc/ssh/sshd_config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root login on ssh no longer allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good program: programs you would like installed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goodprogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libpam-pwquality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libpam-pwquality installed for password complexity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad program: programs you would like removed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">badprogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydra has been removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group to be added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groupadded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patrol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group patrol has been created.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group to be removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groupremoved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nine-eight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group nine-eight has been removed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program to check version of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version being scored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">programversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:2.7.4-0ubuntu1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path to forensics question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer to the question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkforensics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/jperalta/Desktop/forensics1.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tjeffords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forensics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forensics 1 answered correctly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/jperalta/Desktop/forensics2.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">detectives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forensics 2 answered correctly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency of check (0, 1, 2, 7, or 14) days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check4updates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workstation checking for updates daily.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for auto installing updates (0 = no, 1 = yes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updateautoinstall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workstation automatically installing updates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User to look for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group to look in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">useringroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rholt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User rholt is now an administrator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usernotingroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glinetti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User glinetti is no longer an administrator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User with the empty password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emptypassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cboyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insecure password for user cboyle has been changed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service/process that you want stopped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">badprocess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apache2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service apache2 is no longer running.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service/process that should be running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goodprocess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sshd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service sshd is running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File to check permissions of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permissions should NOT be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permnotequalto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-rw-rw-rw-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/etc/ssh/sshd_config permissions secured.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permissions SHOULD be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permequalto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/etc/shadow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-rw-r-----</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/etc/shadow permissions secured.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File that should be deleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">badfile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/asantiago/Videos/jake.mov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscellaneous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unauthorized media file removed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial kernel version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kernelupdated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.15.0-57-generic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kernel updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String to remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removefromcron</t>
+  </si>
+  <si>
     <t xml:space="preserve">jperalta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Essential user has been removed!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Users who should be added.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newuser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nscully</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User nscully has been added.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To disable this, delete the entire row below</t>
-  </si>
-  <si>
-    <t xml:space="preserve">checkfirewall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security Policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Firewall is enabled.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text to remove</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#File to remove it from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">removefromfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allow-guest=true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/etc/lightdm/lightdm.conf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guest account disabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text to add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#File to add it to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addtofile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PermitRootLogin no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/etc/ssh/sshd_config</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Root login on ssh no longer allowed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good program: programs you would like installed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goodprogram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">libpam-pwquality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Program Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libpam-pwquality installed for password complexity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bad program: programs you would like removed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">badprogram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hydra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydra has been removed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group to be added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">groupadded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group patrol has been created.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group to be removed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">groupremoved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nine-eight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group nine-eight has been removed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Program to check version of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version being scored</t>
-  </si>
-  <si>
-    <t xml:space="preserve">programversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1:2.7.4-0ubuntu1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git updated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path to forensics question</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer to the question</t>
-  </si>
-  <si>
-    <t xml:space="preserve">checkforensics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/jperalta/Desktop/forensics1.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tjeffords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forensics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forensics 1 answered correctly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/jperalta/Desktop/forensics2.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">detectives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forensics 2 answered correctly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frequency of check (0, 1, 2, 7, or 14) days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check4updates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workstation checking for updates daily.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check for auto installing updates (0 = no, 1 = yes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">updateautoinstall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workstation automatically installing updates.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User to look for</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group to look in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">useringroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rholt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sudo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User rholt is now an administrator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usernotingroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glinetti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User glinetti is no longer an administrator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User with the empty password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emptypassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cboyle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insecure password for user cboyle has been changed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service/process that you want stopped</t>
-  </si>
-  <si>
-    <t xml:space="preserve">badprocess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apache2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service apache2 is no longer running.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service/process that should be running</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goodprocess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sshd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service sshd is running</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File to check permissions of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permissions should NOT be</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permnotequalto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-rw-rw-rw-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/etc/ssh/sshd_config permissions secured.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permissions SHOULD be</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permequalto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/etc/shadow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-rw-r-----</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/etc/shadow permissions secured.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File that should be deleted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">badfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/asantiago/Videos/jake.mov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miscellaneous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unauthorized media file removed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial kernel version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kernelupdated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.15.0-57-generic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kernel updated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String to remove</t>
-  </si>
-  <si>
-    <t xml:space="preserve">removefromcron</t>
   </si>
   <si>
     <t xml:space="preserve">hello</t>
@@ -587,19 +590,19 @@
   </sheetPr>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="54.64"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1505,10 +1508,10 @@
         <v>116</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>108</v>
@@ -1517,7 +1520,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,13 +1543,13 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>108</v>
@@ -1555,7 +1558,7 @@
         <v>7</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,7 +1566,7 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
@@ -1585,13 +1588,13 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E53" s="2" t="n">
         <v>10</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
@@ -1617,23 +1620,23 @@
         <v>87</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>10</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Changed emptypassword to weakpassword (new regex)
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -271,7 +271,7 @@
     <t xml:space="preserve">User with the empty password</t>
   </si>
   <si>
-    <t xml:space="preserve">emptypassword</t>
+    <t xml:space="preserve">weakpassword</t>
   </si>
   <si>
     <t xml:space="preserve">cboyle</t>
@@ -590,19 +590,19 @@
   </sheetPr>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,7 +1636,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>